<commit_message>
Added filter functionality for categories
</commit_message>
<xml_diff>
--- a/distribuicao.xlsx
+++ b/distribuicao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efaba16bd2b79c6e/pytho_2/Presuposto/analise_presuposto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diegoV\Documents\GitHub\dash_presupost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{0A653156-ADA3-4FD0-B92A-7FE5E3143E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49FE14D0-0509-47EF-B85A-4118C3399D5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DD0C92-1B01-4A10-856D-BF85A59A917C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26895" yWindow="2520" windowWidth="28200" windowHeight="14370" xr2:uid="{7DF961D9-9F94-4B2C-8B12-D53E130C82E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7DF961D9-9F94-4B2C-8B12-D53E130C82E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Exp. Acc</t>
   </si>
   <si>
-    <t>Instituição</t>
-  </si>
-  <si>
     <t>Organ</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>CY23 Others BUDGET</t>
+  </si>
+  <si>
+    <t>Institution</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -896,9 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D13EA72-652C-4619-8DCC-0698ED9B9B83}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -934,48 +932,48 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
       </c>
       <c r="G2">
         <v>47466.079999999994</v>
@@ -992,22 +990,22 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>1059462</v>
@@ -1021,22 +1019,22 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
       </c>
       <c r="G4">
         <v>2532.9</v>
@@ -1053,22 +1051,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>66814</v>
@@ -1082,22 +1080,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
       </c>
       <c r="H6">
         <v>35125</v>
@@ -1111,22 +1109,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7">
         <v>155717</v>
@@ -1140,22 +1138,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
       </c>
       <c r="G8">
         <v>214.94</v>
@@ -1172,22 +1170,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9">
         <v>5601</v>
@@ -1201,22 +1199,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
       </c>
       <c r="H10">
         <v>10000</v>
@@ -1230,22 +1228,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1256,22 +1254,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12">
         <v>31036</v>
@@ -1285,22 +1283,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
       <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
         <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
       </c>
       <c r="H13">
         <v>57000</v>
@@ -1314,22 +1312,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
       </c>
       <c r="H14">
         <v>10000</v>
@@ -1343,22 +1341,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1369,22 +1367,22 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
       <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
         <v>14</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
       </c>
       <c r="G16">
         <v>134.19</v>
@@ -1401,22 +1399,22 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17">
         <v>4084.43</v>
@@ -1430,22 +1428,22 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18">
         <v>1200</v>
@@ -1459,22 +1457,22 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19">
         <v>27956</v>
@@ -1488,22 +1486,22 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
         <v>54</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" t="s">
-        <v>55</v>
       </c>
       <c r="H20">
         <v>14210</v>
@@ -1517,22 +1515,22 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21">
         <v>17361.739999999998</v>
@@ -1546,22 +1544,22 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>59</v>
-      </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22">
         <v>948.4</v>
@@ -1575,22 +1573,22 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>61</v>
-      </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1604,22 +1602,22 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1633,22 +1631,22 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
         <v>64</v>
       </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
       <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>14</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
       </c>
       <c r="H25">
         <v>4070</v>
@@ -1665,22 +1663,22 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
         <v>66</v>
       </c>
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>67</v>
-      </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26">
         <v>27000</v>
@@ -1697,22 +1695,22 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
         <v>68</v>
       </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I27">
         <v>24053</v>
@@ -1729,22 +1727,22 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
-      </c>
       <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
         <v>14</v>
-      </c>
-      <c r="F28" t="s">
-        <v>15</v>
       </c>
       <c r="H28">
         <v>34500</v>
@@ -1761,22 +1759,22 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
-      </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J29">
         <v>115324</v>
@@ -1790,22 +1788,22 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
         <v>74</v>
       </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
-      </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J30">
         <v>122227.87</v>
@@ -1819,22 +1817,22 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
         <v>76</v>
       </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>77</v>
-      </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -1848,22 +1846,22 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" t="s">
-        <v>79</v>
-      </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J32">
         <v>56120.35</v>
@@ -1877,22 +1875,22 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" t="s">
-        <v>81</v>
-      </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J33">
         <v>44587.58</v>
@@ -1906,22 +1904,22 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
         <v>78</v>
       </c>
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
-      </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1938,22 +1936,22 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="B35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" t="s">
-        <v>83</v>
-      </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I35">
         <v>54021</v>
@@ -1970,22 +1968,22 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
         <v>84</v>
       </c>
-      <c r="B36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>85</v>
-      </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36">
         <v>13367.66</v>
@@ -1999,22 +1997,22 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" t="s">
         <v>86</v>
       </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
-      </c>
       <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
         <v>14</v>
-      </c>
-      <c r="F37" t="s">
-        <v>15</v>
       </c>
       <c r="H37">
         <v>4762</v>
@@ -2031,22 +2029,22 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" t="s">
-        <v>89</v>
-      </c>
       <c r="E38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2060,22 +2058,22 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
         <v>90</v>
       </c>
-      <c r="B39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
-      </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J39">
         <v>5759.12</v>
@@ -2089,22 +2087,22 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
         <v>92</v>
       </c>
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" t="s">
-        <v>93</v>
-      </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J40">
         <v>352.42</v>
@@ -2118,22 +2116,22 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" t="s">
         <v>94</v>
       </c>
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" t="s">
-        <v>95</v>
-      </c>
       <c r="E41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2150,22 +2148,22 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
         <v>96</v>
       </c>
-      <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" t="s">
-        <v>97</v>
-      </c>
       <c r="E42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I42">
         <v>53560</v>
@@ -2182,22 +2180,22 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
         <v>98</v>
       </c>
-      <c r="B43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>99</v>
       </c>
-      <c r="D43" t="s">
-        <v>100</v>
-      </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H43">
         <v>3500</v>
@@ -2214,22 +2212,22 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
         <v>101</v>
       </c>
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
-      </c>
       <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
         <v>14</v>
-      </c>
-      <c r="F44" t="s">
-        <v>15</v>
       </c>
       <c r="H44">
         <v>12000</v>
@@ -2246,22 +2244,22 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
         <v>103</v>
       </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>104</v>
-      </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J45">
         <v>2496.8599999999997</v>
@@ -2275,22 +2273,22 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
         <v>105</v>
       </c>
-      <c r="B46" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>106</v>
       </c>
-      <c r="D46" t="s">
-        <v>107</v>
-      </c>
       <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
         <v>14</v>
-      </c>
-      <c r="F46" t="s">
-        <v>15</v>
       </c>
       <c r="G46">
         <v>2500</v>
@@ -2307,22 +2305,22 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J47">
         <v>1809.99</v>
@@ -2336,22 +2334,22 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
         <v>110</v>
       </c>
-      <c r="B48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" t="s">
-        <v>111</v>
-      </c>
       <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
         <v>14</v>
-      </c>
-      <c r="F48" t="s">
-        <v>15</v>
       </c>
       <c r="H48">
         <v>3800</v>
@@ -2368,22 +2366,22 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" t="s">
         <v>112</v>
       </c>
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" t="s">
-        <v>113</v>
-      </c>
       <c r="E49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J49">
         <v>21735.98</v>
@@ -2397,22 +2395,22 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
         <v>114</v>
       </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" t="s">
-        <v>115</v>
-      </c>
       <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
         <v>14</v>
-      </c>
-      <c r="F50" t="s">
-        <v>15</v>
       </c>
       <c r="H50">
         <v>1200</v>
@@ -2429,22 +2427,22 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
         <v>116</v>
       </c>
-      <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" t="s">
-        <v>117</v>
-      </c>
       <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
         <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>15</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -2458,22 +2456,22 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
         <v>118</v>
       </c>
-      <c r="B52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" t="s">
-        <v>106</v>
-      </c>
-      <c r="D52" t="s">
-        <v>119</v>
-      </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J52">
         <v>53416</v>
@@ -2487,22 +2485,22 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" t="s">
         <v>120</v>
       </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>106</v>
-      </c>
-      <c r="D53" t="s">
-        <v>121</v>
-      </c>
       <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
         <v>14</v>
-      </c>
-      <c r="F53" t="s">
-        <v>15</v>
       </c>
       <c r="H53">
         <v>32500</v>
@@ -2519,22 +2517,22 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" t="s">
         <v>122</v>
       </c>
-      <c r="B54" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D54" t="s">
-        <v>123</v>
-      </c>
       <c r="E54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J54">
         <v>44630.91</v>
@@ -2548,22 +2546,22 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" t="s">
         <v>124</v>
       </c>
-      <c r="B55" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" t="s">
-        <v>125</v>
-      </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J55">
         <v>218.67</v>
@@ -2577,22 +2575,22 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" t="s">
         <v>126</v>
       </c>
-      <c r="B56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" t="s">
-        <v>127</v>
-      </c>
       <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
         <v>14</v>
-      </c>
-      <c r="F56" t="s">
-        <v>15</v>
       </c>
       <c r="H56">
         <v>11500</v>
@@ -2609,22 +2607,22 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" t="s">
         <v>128</v>
       </c>
-      <c r="B57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" t="s">
-        <v>106</v>
-      </c>
-      <c r="D57" t="s">
-        <v>129</v>
-      </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I57">
         <v>7960</v>
@@ -2641,22 +2639,22 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" t="s">
         <v>130</v>
       </c>
-      <c r="B58" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" t="s">
-        <v>106</v>
-      </c>
-      <c r="D58" t="s">
-        <v>131</v>
-      </c>
       <c r="E58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J58">
         <v>7929.03</v>
@@ -2670,22 +2668,22 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
         <v>132</v>
       </c>
-      <c r="B59" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>133</v>
       </c>
-      <c r="D59" t="s">
-        <v>134</v>
-      </c>
       <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
         <v>14</v>
-      </c>
-      <c r="F59" t="s">
-        <v>15</v>
       </c>
       <c r="G59">
         <v>20000</v>
@@ -2705,22 +2703,22 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" t="s">
         <v>135</v>
       </c>
-      <c r="B60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" t="s">
-        <v>133</v>
-      </c>
-      <c r="D60" t="s">
-        <v>136</v>
-      </c>
       <c r="E60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J60">
         <v>314.20999999999998</v>
@@ -2734,22 +2732,22 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" t="s">
         <v>137</v>
       </c>
-      <c r="B61" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" t="s">
-        <v>138</v>
-      </c>
       <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
         <v>14</v>
-      </c>
-      <c r="F61" t="s">
-        <v>15</v>
       </c>
       <c r="H61">
         <v>13000</v>
@@ -2766,22 +2764,22 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" t="s">
         <v>139</v>
       </c>
-      <c r="B62" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" t="s">
-        <v>133</v>
-      </c>
-      <c r="D62" t="s">
-        <v>140</v>
-      </c>
       <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
         <v>14</v>
-      </c>
-      <c r="F62" t="s">
-        <v>15</v>
       </c>
       <c r="H62">
         <v>63825</v>
@@ -2798,22 +2796,22 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" t="s">
         <v>141</v>
       </c>
-      <c r="B63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" t="s">
-        <v>133</v>
-      </c>
-      <c r="D63" t="s">
-        <v>142</v>
-      </c>
       <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
         <v>14</v>
-      </c>
-      <c r="F63" t="s">
-        <v>15</v>
       </c>
       <c r="H63">
         <v>4000</v>
@@ -2830,22 +2828,22 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" t="s">
         <v>143</v>
       </c>
-      <c r="B64" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" t="s">
-        <v>144</v>
-      </c>
       <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
         <v>14</v>
-      </c>
-      <c r="F64" t="s">
-        <v>15</v>
       </c>
       <c r="H64">
         <v>13000</v>
@@ -2862,22 +2860,22 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
         <v>145</v>
       </c>
-      <c r="B65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" t="s">
-        <v>133</v>
-      </c>
-      <c r="D65" t="s">
-        <v>146</v>
-      </c>
       <c r="E65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J65">
         <v>35187.08</v>
@@ -2891,22 +2889,22 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
         <v>147</v>
       </c>
-      <c r="B66" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>148</v>
       </c>
-      <c r="D66" t="s">
-        <v>149</v>
-      </c>
       <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s">
         <v>14</v>
-      </c>
-      <c r="F66" t="s">
-        <v>15</v>
       </c>
       <c r="H66">
         <v>1500</v>
@@ -2923,22 +2921,22 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" t="s">
         <v>150</v>
       </c>
-      <c r="B67" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" t="s">
-        <v>151</v>
-      </c>
       <c r="E67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J67">
         <v>11921.01</v>
@@ -2952,22 +2950,22 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" t="s">
         <v>152</v>
       </c>
-      <c r="B68" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" t="s">
-        <v>153</v>
-      </c>
       <c r="E68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I68">
         <v>20950</v>
@@ -2984,22 +2982,22 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C69" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" t="s">
         <v>154</v>
       </c>
-      <c r="B69" t="s">
-        <v>53</v>
-      </c>
-      <c r="C69" t="s">
-        <v>148</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" t="s">
         <v>155</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" t="s">
-        <v>156</v>
       </c>
       <c r="G69">
         <v>4000</v>
@@ -3019,22 +3017,22 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" t="s">
         <v>157</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" t="s">
         <v>158</v>
       </c>
-      <c r="C70" t="s">
-        <v>148</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" t="s">
         <v>159</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" t="s">
-        <v>160</v>
       </c>
       <c r="G70">
         <v>6000</v>
@@ -3054,22 +3052,22 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>160</v>
+      </c>
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" t="s">
         <v>161</v>
       </c>
-      <c r="B71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" t="s">
-        <v>148</v>
-      </c>
-      <c r="D71" t="s">
-        <v>162</v>
-      </c>
       <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" t="s">
         <v>14</v>
-      </c>
-      <c r="F71" t="s">
-        <v>15</v>
       </c>
       <c r="H71">
         <v>1500</v>
@@ -3086,22 +3084,22 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>162</v>
+      </c>
+      <c r="B72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" t="s">
         <v>163</v>
       </c>
-      <c r="B72" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" t="s">
-        <v>148</v>
-      </c>
-      <c r="D72" t="s">
-        <v>164</v>
-      </c>
       <c r="E72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I72">
         <v>3000</v>
@@ -3118,22 +3116,22 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" t="s">
         <v>165</v>
       </c>
-      <c r="B73" t="s">
-        <v>158</v>
-      </c>
-      <c r="C73" t="s">
-        <v>148</v>
-      </c>
-      <c r="D73" t="s">
-        <v>166</v>
-      </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G73">
         <v>28539</v>

</xml_diff>